<commit_message>
change country USA to United States
</commit_message>
<xml_diff>
--- a/input_data_spreadsheet/Port_Country.xlsx
+++ b/input_data_spreadsheet/Port_Country.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="249">
   <si>
     <t xml:space="preserve">port</t>
   </si>
@@ -127,397 +127,400 @@
     <t xml:space="preserve">Baton Rouge</t>
   </si>
   <si>
+    <t xml:space="preserve">United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batumi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Georgia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bayport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaumont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beirut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lebanon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bejaia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilbao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bizerte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tunisia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonga Offshore Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonny Offshore Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brisbane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burgas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bulgaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPC Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russian Federation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cartagena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colombia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castellon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ceyhan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clov FPSO / Cravo, Lirio, Orquidea and Violeta Fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copenhagen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corpus Christi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dalia FPSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damietta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Arab Emirates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Djeno Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dortyol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dos Bocas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ebok Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egina Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Dekheila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Ferrol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eleusis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es Sider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escravos Oil Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farwah Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flotta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forcados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fredericia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freeport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fujairah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galveston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gibraltar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girassol Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goteborg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haifa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Israel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Houston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ima Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamnagar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jubail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saudi Arabia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalamaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalundborg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kharg Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klaipeda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithuania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kulevi Oil Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwangyang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korea South</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOOP Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Coruna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Skhirra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las Palmas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le Havre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leixoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portugal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limassol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyprus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marsa Bashayer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marsa el Brega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marsa el Hariga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marsaxlokk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mellitah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mersa el Hamra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mersin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mina Abdullah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuwait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mina Al Ahmadi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mina Saqr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mongstad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moudi Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cameroon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murmansk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nemrut Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Mangalore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nikolayev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukraine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novorossiysk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odessa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odudu Terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pazflor Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piraeus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pointe Noire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Arthur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Gentil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Rashid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Sulphur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port de Bouc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primorsk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rabigh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ras Laffan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ras Lanuf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ras Tanura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserve</t>
+  </si>
+  <si>
     <t xml:space="preserve">USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Batumi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Georgia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bayport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beaumont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beirut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lebanon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bejaia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bilbao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bizerte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tunisia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonga Offshore Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonny Offshore Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bouri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brisbane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burgas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bulgaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPC Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Russian Federation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cadiz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cartagena</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colombia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Castellon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ceyhan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clov FPSO / Cravo, Lirio, Orquidea and Violeta Fields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copenhagen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denmark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corpus Christi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dalia FPSO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Damietta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Das Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Arab Emirates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Djeno Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Congo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dortyol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dos Bocas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mexico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Albania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ebok Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egina Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El Dekheila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El Ferrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eleusis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es Sider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escravos Oil Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farwah Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flotta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forcados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fredericia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Freeport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fujairah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Galveston</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gibraltar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Girassol Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goteborg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sweden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haifa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Israel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Houston</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ima Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jamnagar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jubail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saudi Arabia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalamaki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalundborg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kharg Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Klaipeda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lithuania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kulevi Oil Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kwangyang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Korea South</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOOP Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La Coruna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La Skhirra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las Palmas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le Havre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leixoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portugal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limassol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyprus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marsa Bashayer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sudan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marsa el Brega</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marsa el Hariga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marsaxlokk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mellitah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mersa el Hamra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mersin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mina Abdullah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kuwait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mina Al Ahmadi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mina Saqr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mongstad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moudi Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cameroon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Murmansk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nemrut Bay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Mangalore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nikolayev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ukraine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Novorossiysk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Odessa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Odudu Terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pazflor Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piraeus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pointe Noire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port Arthur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port Gentil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gabon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port Rashid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port Sudan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port Sulphur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port de Bouc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primorsk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rabigh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ras Laffan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qatar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ras Lanuf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ras Tanura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reserve</t>
   </si>
   <si>
     <t xml:space="preserve">Rijeka</t>
@@ -965,8 +968,8 @@
   </sheetPr>
   <dimension ref="A1:B193"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B150" activeCellId="0" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1932,12 +1935,12 @@
         <v>164</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>34</v>
+        <v>165</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>29</v>
@@ -1945,7 +1948,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>74</v>
@@ -1953,7 +1956,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>17</v>
@@ -1961,15 +1964,15 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>67</v>
@@ -1977,15 +1980,15 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>15</v>
@@ -1993,7 +1996,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>60</v>
@@ -2001,7 +2004,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>84</v>
@@ -2009,7 +2012,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>11</v>
@@ -2017,7 +2020,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>101</v>
@@ -2025,15 +2028,15 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>118</v>
@@ -2041,7 +2044,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>21</v>
@@ -2049,7 +2052,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>135</v>
@@ -2057,7 +2060,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>84</v>
@@ -2065,15 +2068,15 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>34</v>
@@ -2081,7 +2084,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>53</v>
@@ -2089,7 +2092,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>62</v>
@@ -2097,15 +2100,15 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>11</v>
@@ -2113,7 +2116,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>84</v>
@@ -2121,7 +2124,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>36</v>
@@ -2129,15 +2132,15 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>53</v>
@@ -2145,7 +2148,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>13</v>
@@ -2153,7 +2156,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>84</v>
@@ -2161,7 +2164,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>34</v>
@@ -2169,7 +2172,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>8</v>
@@ -2177,7 +2180,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>24</v>
@@ -2185,7 +2188,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>53</v>
@@ -2193,7 +2196,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>15</v>
@@ -2201,7 +2204,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>53</v>
@@ -2209,7 +2212,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>101</v>
@@ -2217,7 +2220,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>120</v>
@@ -2225,7 +2228,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>53</v>
@@ -2233,23 +2236,23 @@
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>103</v>
@@ -2257,15 +2260,15 @@
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>15</v>
@@ -2273,15 +2276,15 @@
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>8</v>
@@ -2289,7 +2292,7 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>24</v>
@@ -2297,226 +2300,226 @@
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>